<commit_message>
Clusters are treated correctly now.
</commit_message>
<xml_diff>
--- a/atores_relacoes.xlsx
+++ b/atores_relacoes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luiz/Documents/CDEM 2020/E3/Planejamento Operativo/Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luiz/Documents/Python/relationshipdiagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5BB0C3-C9D3-BC4F-A1EF-25C493E11DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F41916-5D18-E347-8005-9363DDD7413E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{C6D7EF91-DF44-AD45-98A8-8811F9299FCF}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="47">
   <si>
     <t>Tipos</t>
   </si>
@@ -172,7 +172,7 @@
     <t>Cortou Rel\ndiplomáticas</t>
   </si>
   <si>
-    <t>Tharcio</t>
+    <t>Busca relações diplomáticas</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,10 +746,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
@@ -759,6 +756,12 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
       <c r="N11" s="10" t="s">
         <v>42</v>
       </c>
@@ -781,7 +784,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1152,16 +1155,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
loop para mais de um arquivo
Acrescentado um loop para fazer um diagrama para cada arquivo xlsx na pasta.

Acrescentado tratamento de exceção para falha na abertura de arquivo.
</commit_message>
<xml_diff>
--- a/atores_relacoes.xlsx
+++ b/atores_relacoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luiz/Documents/CDEM 2020/E3/Planejamento Operativo/GT2/Avaliação Integradora/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\python\relationshipdiagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247D54AB-B454-9D40-889E-FBBE3C667D9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B207C51-037F-4071-8A28-F8F6CDA96167}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="1110" windowWidth="25815" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atores" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="45">
   <si>
     <t>ator</t>
   </si>
@@ -158,13 +158,16 @@
   </si>
   <si>
     <t>Patrocina</t>
+  </si>
+  <si>
+    <t>Branco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,6 +187,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -275,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -290,6 +300,9 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,50 +518,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N997"/>
+  <dimension ref="A1:H997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A13" sqref="A13:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
     <col min="4" max="26" width="11" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="11.28515625" style="2"/>
+    <col min="27" max="16384" width="11.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="H1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -558,11 +571,11 @@
       <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -572,11 +585,11 @@
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -586,11 +599,11 @@
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -600,65 +613,69 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="H6" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1" t="s">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="H9" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
@@ -666,13 +683,13 @@
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N11" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
@@ -680,33 +697,22 @@
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1757,7 +1763,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B48" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$N$2:$N$11</formula1>
+      <formula1>$H$2:$H$12</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
@@ -1770,31 +1776,31 @@
   <dimension ref="A1:O852"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
     <col min="3" max="26" width="11" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="11.28515625" style="2"/>
+    <col min="27" max="16384" width="11.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -3088,10 +3094,10 @@
     <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D28:D50" xr:uid="{E96F2FD8-7DF2-A74F-AB20-2B59CC82A28D}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D50" xr:uid="{E96F2FD8-7DF2-A74F-AB20-2B59CC82A28D}">
       <formula1>$N$2:$N$4</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E28:E50" xr:uid="{96294DC5-1B78-0144-8CE6-CD7EB3BCA6E0}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E50" xr:uid="{96294DC5-1B78-0144-8CE6-CD7EB3BCA6E0}">
       <formula1>$O$2:$O$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -3099,18 +3105,12 @@
   <pageSetup orientation="landscape"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{26495AA4-94C2-D942-858E-3803A692795A}">
           <x14:formula1>
             <xm:f>atores!$A$2:$A$50</xm:f>
           </x14:formula1>
-          <xm:sqref>A28:A50</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{CB21DD55-9CE2-2148-9830-CE4F5854392D}">
-          <x14:formula1>
-            <xm:f>atores!$A$3:$A$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>C28:C50</xm:sqref>
+          <xm:sqref>A2:A50 C2:C50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>